<commit_message>
few extra key name / values included in vfm analysis
</commit_message>
<xml_diff>
--- a/tests/resources/test_vfm_master_1_2020.xlsx
+++ b/tests/resources/test_vfm_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="108">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -338,6 +338,12 @@
   </si>
   <si>
     <t xml:space="preserve">Rail Group</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Benefits Narrative </t>
+  </si>
+  <si>
+    <t xml:space="preserve">All you need is love, love is all you need </t>
   </si>
 </sst>
 </file>
@@ -421,7 +427,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -435,6 +441,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -460,7 +470,7 @@
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A52" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="A70" activeCellId="0" sqref="70:70"/>
+      <selection pane="bottomLeft" activeCell="C71" activeCellId="0" sqref="C71"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1479,6 +1489,14 @@
       <c r="ALE70" s="1"/>
       <c r="ALF70" s="1"/>
       <c r="ALG70" s="1"/>
+    </row>
+    <row r="71" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B71" s="1" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="1046075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1046076" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>

<commit_message>
vfm class refactored to latest data structure
</commit_message>
<xml_diff>
--- a/tests/resources/test_vfm_master_1_2020.xlsx
+++ b/tests/resources/test_vfm_master_1_2020.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="110">
   <si>
     <t xml:space="preserve">Project/Programme Name</t>
   </si>
@@ -347,6 +347,9 @@
   </si>
   <si>
     <t xml:space="preserve">All you need is love, love is all you need </t>
+  </si>
+  <si>
+    <t xml:space="preserve">GMPP - IPA ID Number</t>
   </si>
 </sst>
 </file>
@@ -476,9 +479,9 @@
   <dimension ref="A1:ALG1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="74" zoomScaleNormal="74" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A25" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A63" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="D57" activeCellId="0" sqref="D57"/>
+      <selection pane="bottomLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="13.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1504,6 +1507,11 @@
       </c>
       <c r="B71" s="1" t="s">
         <v>108</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="1046075" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>

</xml_diff>